<commit_message>
testing alternatives to the RAG system
</commit_message>
<xml_diff>
--- a/support_files/testing_queries.xlsx
+++ b/support_files/testing_queries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\estaciolima\pdf_reader\support_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D836D39A-C2D0-43A5-ACC5-CF9D3AC00787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE5541A-9865-4BFD-BB91-156BDB7F1D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{6FA36C75-6DEA-49C0-A516-63D137A7F56D}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="21090" xr2:uid="{6FA36C75-6DEA-49C0-A516-63D137A7F56D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,19 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Can I use my phone as a key for this car?</t>
-  </si>
-  <si>
-    <t>Does the user manual mention a smartphone key feature for this model?</t>
-  </si>
-  <si>
-    <t>What are the steps to start the engine in this car?</t>
-  </si>
-  <si>
-    <t>How do I use the push-button start feature, if available, in this vehicle?</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>What does the manual say about turning on the engine with or without a key?</t>
   </si>
@@ -62,25 +50,31 @@
     <t>What are the instructions in the manual for setting up memory seats?</t>
   </si>
   <si>
-    <t>What are the steps for adjusting the side and rear-view mirrors in my car?</t>
-  </si>
-  <si>
-    <t>How can I manually or electronically adjust the mirrors in this vehicle?</t>
-  </si>
-  <si>
-    <t>Is there a specific section in the manual about mirror adjustments?</t>
-  </si>
-  <si>
-    <t>What is the procedure for adjusting the braking system or pedal sensitivity?</t>
-  </si>
-  <si>
-    <t>How do I ensure the brakes are correctly adjusted for optimal performance?</t>
-  </si>
-  <si>
-    <t>What does the manual say about maintaining and adjusting the brakes?</t>
-  </si>
-  <si>
     <t>query</t>
+  </si>
+  <si>
+    <t>How do I use my smartphone to unlock the car?</t>
+  </si>
+  <si>
+    <t>How do I use my phone to open the car?</t>
+  </si>
+  <si>
+    <t>I want to enter my car using my phone.</t>
+  </si>
+  <si>
+    <t>How do I disarm the vehicle security system?</t>
+  </si>
+  <si>
+    <t>Who is Michael Jackson?</t>
+  </si>
+  <si>
+    <t>Who can I adjust my steering wheel column?</t>
+  </si>
+  <si>
+    <t>Who can I adjust my steering column?</t>
+  </si>
+  <si>
+    <t>Can you give me an overview of the features in this vehicle?</t>
   </si>
 </sst>
 </file>
@@ -116,9 +110,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,88 +446,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7086D0-69A3-42D6-BEEC-660C19552CE6}">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="63.77734375" customWidth="1"/>
+    <col min="1" max="1" width="63.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>